<commit_message>
ReusableComponent Code Updated as per PageFactory
</commit_message>
<xml_diff>
--- a/src/test/resources/com/jtaf/excel/testData.xlsx
+++ b/src/test/resources/com/jtaf/excel/testData.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumPageObjectModelFramework\src\test\resources\com\jtaf\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5904303A-C876-43B6-85EE-53CC27CE9710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D2CA21-4CCC-4A21-95AD-84F4D8C71419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId2"/>
-    <sheet name="AdminPageTest" sheetId="2" r:id="rId3"/>
+    <sheet name="PFLoginPageTest" sheetId="4" r:id="rId3"/>
+    <sheet name="AdminPageTest" sheetId="2" r:id="rId4"/>
+    <sheet name="PFAdminPageTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -63,6 +65,12 @@
   </si>
   <si>
     <t>SearchCriteria</t>
+  </si>
+  <si>
+    <t>PFLoginPageTest</t>
+  </si>
+  <si>
+    <t>PFAdminPageTest</t>
   </si>
 </sst>
 </file>
@@ -403,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,6 +443,22 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -485,7 +509,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB614EB-60E5-4D7E-A974-9B93504FA296}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C39480-F02B-40BC-AAFB-DAA923AC03BA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
PageFactory Code Updated and Working Fine
</commit_message>
<xml_diff>
--- a/src/test/resources/com/jtaf/excel/testData.xlsx
+++ b/src/test/resources/com/jtaf/excel/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumPageObjectModelFramework\src\test\resources\com\jtaf\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D2CA21-4CCC-4A21-95AD-84F4D8C71419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEEAC8E-3CDF-4CCC-BAF2-44ACE3EAFACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId2"/>
     <sheet name="PFLoginPageTest" sheetId="4" r:id="rId3"/>
-    <sheet name="AdminPageTest" sheetId="2" r:id="rId4"/>
-    <sheet name="PFAdminPageTest" sheetId="5" r:id="rId5"/>
+    <sheet name="AdminPageTest" sheetId="5" r:id="rId4"/>
+    <sheet name="PFAdminPageTest" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -513,7 +513,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C39480-F02B-40BC-AAFB-DAA923AC03BA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -584,30 +584,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C39480-F02B-40BC-AAFB-DAA923AC03BA}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Soft Assertion Code Updated in TestCase
</commit_message>
<xml_diff>
--- a/src/test/resources/com/jtaf/excel/testData.xlsx
+++ b/src/test/resources/com/jtaf/excel/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumPageObjectModelFramework\src\test\resources\com\jtaf\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEEAC8E-3CDF-4CCC-BAF2-44ACE3EAFACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F4FC2D-D7C4-4275-9C85-F235EF0311D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="PFLoginPageTest" sheetId="4" r:id="rId3"/>
     <sheet name="AdminPageTest" sheetId="5" r:id="rId4"/>
     <sheet name="PFAdminPageTest" sheetId="2" r:id="rId5"/>
+    <sheet name="PFErrorCaptureTest" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -71,6 +72,9 @@
   </si>
   <si>
     <t>PFAdminPageTest</t>
+  </si>
+  <si>
+    <t>PFErrorCaptureTest</t>
   </si>
 </sst>
 </file>
@@ -411,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +463,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -587,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -631,4 +643,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513FE6EA-8523-41A3-A3FE-3120F5994DE4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>